<commit_message>
Add yes/no with comments to Module 7
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_7.xlsx
+++ b/templates/NHWA_Module_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644183BA-0819-4FB5-853E-89D08D822CD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8B329-BD09-40B6-B4CA-2780F2656E4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="w6U6L0oAe3JJA59tHtarEV89NpD3W2+RkrpCLpSky0mah3WxgT5zGiZyUg4WqiEAxmmZBm6plpvj46rywraaLA==" workbookSaltValue="p57C/QL86ueJeh1bq5eaXQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2761,10 +2761,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2794,6 +2790,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -10305,7 +10305,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:O20"/>
+  <dimension ref="B1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -10318,11 +10318,10 @@
     <col min="3" max="3" width="53.42578125" style="3" customWidth="1"/>
     <col min="4" max="9" width="15.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="10" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="20" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="3" hidden="1" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -10413,36 +10412,36 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="42" t="s">
         <v>790</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="45" t="s">
         <v>777</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="52" t="s">
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="51" t="s">
         <v>791</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
     </row>
     <row r="9" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="33" t="s">
         <v>782</v>
       </c>
@@ -10560,8 +10559,8 @@
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="s">
         <v>9</v>
       </c>
@@ -10579,7 +10578,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -10591,27 +10590,27 @@
       <c r="N19" s="11">
         <v>1</v>
       </c>
-      <c r="O19" s="3" t="str">
+    </row>
+    <row r="20" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>778</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="N20" s="3" t="str">
         <f>IF(N19=2,"true",IF(N19=3,"false",""))</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
-        <v>1</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>778</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="TbEEyb7UFTF/HQPN3kRBPG4sYtEV/dub4YGzIad8QwR8axpli+Y9K48SNHGRUBAR+ReR2J0HCdu+vxoy9OwP6w==" saltValue="9UNgL5ts/0WPK1FNlLG1cw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="05Rm/4WzXZZgAOc1yBS2U2YJhWTgszzRDoqQdYLZUmppPeOE3bXYM6vvyKPG2aqq0mIlP8WluvOAgEvWMk0YPQ==" saltValue="5kq9V1BZsF8eqmgsiBtG6w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D20" name="Range1_1"/>
   </protectedRanges>

</xml_diff>